<commit_message>
Add level randomization, rename 'to_block' -> 'render'
</commit_message>
<xml_diff>
--- a/datapacks/Noodle Game/turn_logic.xlsx
+++ b/datapacks/Noodle Game/turn_logic.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benkr\Documents\Minecraft\Laptop\saves\noodles\datapacks\Noodle Game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Minecraft\Personal\saves\Noodles Too\datapacks\Noodle Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6EF512-F0C8-46D4-9870-0551891A0952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D1F39-5C51-43D8-A7F3-E40939B6B5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8376" yWindow="3180" windowWidth="23040" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counter-Clockwise" sheetId="2" r:id="rId1"/>
     <sheet name="Clockwise" sheetId="4" r:id="rId2"/>
+    <sheet name="Flip" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -541,7 +542,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -686,4 +687,158 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129CE2A3-5AE3-49A5-ABBE-F08793A4AAC2}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>